<commit_message>
Added rig start date in Excel file.
</commit_message>
<xml_diff>
--- a/test_case.xlsx
+++ b/test_case.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11105"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\Python\aries_scheduler\with_pad_construction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="239" documentId="5_{EEC16563-7ADD-DF46-9E7F-07DA0F631430}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{1E6A7625-39F8-3543-80AE-CD1628684C08}"/>
+  <xr:revisionPtr revIDLastSave="249" documentId="5_{EEC16563-7ADD-DF46-9E7F-07DA0F631430}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{812A3CB7-DB5C-B34C-A22F-2EE9DF4AB755}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21533" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,6 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="144">
   <si>
     <t>Days MOB In</t>
   </si>
@@ -465,6 +466,9 @@
   </si>
   <si>
     <t>TEST_CASE</t>
+  </si>
+  <si>
+    <t>RIG_START</t>
   </si>
 </sst>
 </file>
@@ -834,12 +838,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:S11" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:S11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:T11" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:T11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="RIG"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PAD"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="STYLE"/>
+    <tableColumn id="20" xr3:uid="{E07EF27C-C01D-CE4F-955A-47FE1BA4BDD1}" name="RIG_START"/>
     <tableColumn id="18" xr3:uid="{6656B175-4140-45E8-A80F-35018ED1682E}" name="PAD_START" dataDxfId="7"/>
     <tableColumn id="19" xr3:uid="{91F04908-A965-4721-BE57-96FFB703D88C}" name="PAD_END" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="CONDUCTORS"/>
@@ -3717,35 +3722,36 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.96484375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.46875" customWidth="1"/>
-    <col min="7" max="7" width="10.4921875" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.23828125" customWidth="1"/>
-    <col min="10" max="10" width="6.72265625" customWidth="1"/>
-    <col min="11" max="11" width="6.45703125" customWidth="1"/>
-    <col min="12" max="12" width="7.53125" customWidth="1"/>
-    <col min="13" max="13" width="13.046875" customWidth="1"/>
-    <col min="14" max="14" width="14.2578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5078125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15.73828125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="14.2578125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="14.52734375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="12.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5078125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.46875" customWidth="1"/>
+    <col min="8" max="8" width="10.4921875" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12.23828125" customWidth="1"/>
+    <col min="11" max="11" width="6.72265625" customWidth="1"/>
+    <col min="12" max="12" width="6.45703125" customWidth="1"/>
+    <col min="13" max="13" width="7.53125" customWidth="1"/>
+    <col min="14" max="14" width="13.046875" customWidth="1"/>
+    <col min="15" max="15" width="14.2578125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5078125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="15.73828125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="14.2578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="14.52734375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="12.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>25</v>
       </c>
@@ -3755,56 +3761,59 @@
       <c r="C1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="R1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="S1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="T1" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -3814,11 +3823,11 @@
       <c r="C2" t="s">
         <v>47</v>
       </c>
-      <c r="P2" s="1">
+      <c r="Q2" s="1">
         <v>43539</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -3828,8 +3837,11 @@
       <c r="C3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D3" s="1">
+        <v>43466</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>95</v>
       </c>
@@ -3840,7 +3852,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -3851,7 +3863,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -3862,7 +3874,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -3872,8 +3884,11 @@
       <c r="C7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D7" s="1">
+        <v>43556</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>96</v>
       </c>
@@ -3884,7 +3899,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>96</v>
       </c>
@@ -3895,7 +3910,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>96</v>
       </c>
@@ -3906,7 +3921,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>96</v>
       </c>

</xml_diff>

<commit_message>
added pods for production start
</commit_message>
<xml_diff>
--- a/test_case.xlsx
+++ b/test_case.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\Python\aries_scheduler\with_pad_construction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="249" documentId="5_{EEC16563-7ADD-DF46-9E7F-07DA0F631430}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{812A3CB7-DB5C-B34C-A22F-2EE9DF4AB755}"/>
+  <xr:revisionPtr revIDLastSave="275" documentId="5_{EEC16563-7ADD-DF46-9E7F-07DA0F631430}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{748656A9-8239-CD4C-BC45-8A41EF85B55D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21533" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21533" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COVER_SHEET" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="145">
   <si>
     <t>Days MOB In</t>
   </si>
@@ -469,6 +469,9 @@
   </si>
   <si>
     <t>RIG_START</t>
+  </si>
+  <si>
+    <t>POD_SIZE</t>
   </si>
 </sst>
 </file>
@@ -838,9 +841,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:T11" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:T11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:U11" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:U11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="RIG"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PAD"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="STYLE"/>
@@ -855,6 +858,7 @@
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="FAC"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="FRAC"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="FLOWBACK"/>
+    <tableColumn id="21" xr3:uid="{6074DCB2-04CB-7148-B517-8D3E4553316A}" name="POD_SIZE"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="DRILL_START" dataDxfId="5"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="DRILL_END" dataDxfId="4"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="COMPL_START" dataDxfId="3"/>
@@ -1165,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H286"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="D3" sqref="D3:G3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1291,7 +1295,7 @@
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
@@ -1321,7 +1325,7 @@
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -1351,7 +1355,7 @@
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -1463,7 +1467,7 @@
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
@@ -1493,7 +1497,7 @@
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -1523,7 +1527,7 @@
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
@@ -3722,10 +3726,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3742,16 +3746,16 @@
     <col min="11" max="11" width="6.72265625" customWidth="1"/>
     <col min="12" max="12" width="6.45703125" customWidth="1"/>
     <col min="13" max="13" width="7.53125" customWidth="1"/>
-    <col min="14" max="14" width="13.046875" customWidth="1"/>
-    <col min="15" max="15" width="14.2578125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5078125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="15.73828125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="14.2578125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="14.52734375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="12.77734375" style="1" customWidth="1"/>
+    <col min="14" max="15" width="13.046875" customWidth="1"/>
+    <col min="16" max="16" width="14.2578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5078125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="15.73828125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="14.2578125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="14.52734375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="12.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>25</v>
       </c>
@@ -3795,25 +3799,28 @@
         <v>16</v>
       </c>
       <c r="O1" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="P1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="R1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="S1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="T1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="U1" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -3823,11 +3830,14 @@
       <c r="C2" t="s">
         <v>47</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
         <v>43539</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -3840,8 +3850,11 @@
       <c r="D3" s="1">
         <v>43466</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>95</v>
       </c>
@@ -3851,8 +3864,11 @@
       <c r="C4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -3862,8 +3878,11 @@
       <c r="C5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -3873,8 +3892,11 @@
       <c r="C6" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -3887,8 +3909,11 @@
       <c r="D7" s="1">
         <v>43556</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>96</v>
       </c>
@@ -3898,8 +3923,11 @@
       <c r="C8" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>96</v>
       </c>
@@ -3909,8 +3937,11 @@
       <c r="C9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>96</v>
       </c>
@@ -3920,8 +3951,11 @@
       <c r="C10" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>96</v>
       </c>
@@ -3930,6 +3964,9 @@
       </c>
       <c r="C11" t="s">
         <v>48</v>
+      </c>
+      <c r="O11">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3949,8 +3986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4065,7 +4102,7 @@
       </c>
       <c r="E3">
         <f>INDEX(COVER_SHEET!$E$7:$E$15,MATCH(INPUTS!E1,COVER_SHEET!$C$7:$C$15,0))</f>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="F3">
         <f>INDEX(COVER_SHEET!$E$7:$E$15,MATCH(INPUTS!F1,COVER_SHEET!$C$7:$C$15,0))</f>
@@ -4073,7 +4110,7 @@
       </c>
       <c r="G3">
         <f>INDEX(COVER_SHEET!$E$7:$E$15,MATCH(INPUTS!G1,COVER_SHEET!$C$7:$C$15,0))</f>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="H3">
         <f>INDEX(COVER_SHEET!$E$7:$E$15,MATCH(INPUTS!H1,COVER_SHEET!$C$7:$C$15,0))</f>
@@ -4081,7 +4118,7 @@
       </c>
       <c r="I3">
         <f>INDEX(COVER_SHEET!$E$7:$E$15,MATCH(INPUTS!I1,COVER_SHEET!$C$7:$C$15,0))</f>
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="J3">
         <f>INDEX(COVER_SHEET!$E$7:$E$15,MATCH(INPUTS!J1,COVER_SHEET!$C$7:$C$15,0))</f>
@@ -4161,7 +4198,7 @@
       </c>
       <c r="E5">
         <f>INDEX(COVER_SHEET!$E$19:$E$27,MATCH(INPUTS!E1,COVER_SHEET!$C$19:$C$27,0))</f>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="F5">
         <f>INDEX(COVER_SHEET!$E$19:$E$27,MATCH(INPUTS!F1,COVER_SHEET!$C$19:$C$27,0))</f>
@@ -4169,7 +4206,7 @@
       </c>
       <c r="G5">
         <f>INDEX(COVER_SHEET!$E$19:$E$27,MATCH(INPUTS!G1,COVER_SHEET!$C$19:$C$27,0))</f>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="H5">
         <f>INDEX(COVER_SHEET!$E$19:$E$27,MATCH(INPUTS!H1,COVER_SHEET!$C$19:$C$27,0))</f>
@@ -4177,7 +4214,7 @@
       </c>
       <c r="I5">
         <f>INDEX(COVER_SHEET!$E$19:$E$27,MATCH(INPUTS!I1,COVER_SHEET!$C$19:$C$27,0))</f>
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="J5">
         <f>INDEX(COVER_SHEET!$E$19:$E$27,MATCH(INPUTS!J1,COVER_SHEET!$C$19:$C$27,0))</f>
@@ -4201,7 +4238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
+    <sheetView workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>

</xml_diff>